<commit_message>
update: dataset taksonomi tumbuhan
</commit_message>
<xml_diff>
--- a/(UPDATE 2) DATA TUMBUHAN TERBARU.xlsx
+++ b/(UPDATE 2) DATA TUMBUHAN TERBARU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praju\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dev\laragon\www\botanica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBCE4DF-DC25-4BD7-83F7-132CFCD3DB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9536290-B4A1-48F5-B4AE-A485401862A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ADBDB189-F3D4-457D-8897-29178EA9F1B5}"/>
   </bookViews>
@@ -23,6 +23,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -5094,20 +5103,20 @@
     <t>titik_koordinat</t>
   </si>
   <si>
-    <t>familly</t>
-  </si>
-  <si>
-    <t>keas</t>
-  </si>
-  <si>
     <t>foto_batang_a</t>
+  </si>
+  <si>
+    <t>kelas</t>
+  </si>
+  <si>
+    <t>family</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5718,11 +5727,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BE4F62-6877-4DC0-ABE6-E26131F42661}">
   <dimension ref="A1:X356"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="2" customWidth="1"/>
@@ -5738,7 +5747,7 @@
     <col min="24" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="85.5" customHeight="1">
+    <row r="1" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5746,7 +5755,7 @@
         <v>1669</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>1688</v>
+        <v>1690</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>1670</v>
@@ -5788,7 +5797,7 @@
         <v>1681</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="R1" s="12" t="s">
         <v>1682</v>
@@ -5809,7 +5818,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="85.5" customHeight="1">
+    <row r="2" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -5852,7 +5861,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="204.75">
+    <row r="3" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -5913,7 +5922,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="141.75">
+    <row r="4" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -5976,7 +5985,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="85.5" customHeight="1">
+    <row r="5" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -6017,7 +6026,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="85.5" customHeight="1">
+    <row r="6" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -6060,7 +6069,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="110.25">
+    <row r="7" spans="1:23" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -6121,7 +6130,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="85.5" customHeight="1">
+    <row r="8" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -6164,7 +6173,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="85.5" customHeight="1">
+    <row r="9" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -6209,7 +6218,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="220.5">
+    <row r="10" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -6274,7 +6283,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="85.5" customHeight="1">
+    <row r="11" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -6317,7 +6326,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="85.5" customHeight="1">
+    <row r="12" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -6358,7 +6367,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="204.75">
+    <row r="13" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -6427,7 +6436,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="85.5" customHeight="1">
+    <row r="14" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -6470,7 +6479,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="85.5" customHeight="1">
+    <row r="15" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -6509,7 +6518,7 @@
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
     </row>
-    <row r="16" spans="1:23" ht="85.5" customHeight="1">
+    <row r="16" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -6548,7 +6557,7 @@
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
     </row>
-    <row r="17" spans="1:23" ht="204.75">
+    <row r="17" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -6611,7 +6620,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="85.5" customHeight="1">
+    <row r="18" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -6652,7 +6661,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="85.5" customHeight="1">
+    <row r="19" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -6693,7 +6702,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="189">
+    <row r="20" spans="1:23" ht="189" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -6756,7 +6765,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="85.5" customHeight="1">
+    <row r="21" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -6795,7 +6804,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="85.5" customHeight="1">
+    <row r="22" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -6834,7 +6843,7 @@
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
     </row>
-    <row r="23" spans="1:23" ht="110.25">
+    <row r="23" spans="1:23" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -6893,7 +6902,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="204.75">
+    <row r="24" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -6960,7 +6969,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="220.5">
+    <row r="25" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -7019,7 +7028,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="85.5" customHeight="1">
+    <row r="26" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -7062,7 +7071,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="204.75">
+    <row r="27" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -7125,7 +7134,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="85.5" customHeight="1">
+    <row r="28" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -7166,7 +7175,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="85.5" customHeight="1">
+    <row r="29" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -7205,7 +7214,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="85.5" customHeight="1">
+    <row r="30" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -7244,7 +7253,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="126">
+    <row r="31" spans="1:23" ht="126" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -7307,7 +7316,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="85.5" customHeight="1">
+    <row r="32" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -7350,7 +7359,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="85.5" customHeight="1">
+    <row r="33" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -7389,7 +7398,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="189">
+    <row r="34" spans="1:23" ht="189" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -7450,7 +7459,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="141.75">
+    <row r="35" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -7513,7 +7522,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="85.5" customHeight="1">
+    <row r="36" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -7554,7 +7563,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="220.5">
+    <row r="37" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -7617,7 +7626,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="85.5" customHeight="1">
+    <row r="38" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -7660,7 +7669,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="85.5" customHeight="1">
+    <row r="39" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -7703,7 +7712,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="85.5" customHeight="1">
+    <row r="40" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -7742,7 +7751,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="85.5" customHeight="1">
+    <row r="41" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -7785,7 +7794,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="204.75">
+    <row r="42" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -7846,7 +7855,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="85.5" customHeight="1">
+    <row r="43" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -7887,7 +7896,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="85.5" customHeight="1">
+    <row r="44" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -7930,7 +7939,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="85.5" customHeight="1">
+    <row r="45" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -7973,7 +7982,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="85.5" customHeight="1">
+    <row r="46" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -8016,7 +8025,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="236.25">
+    <row r="47" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -8077,7 +8086,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="85.5" customHeight="1">
+    <row r="48" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -8120,7 +8129,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="236.25">
+    <row r="49" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -8183,7 +8192,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="85.5" customHeight="1">
+    <row r="50" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -8222,7 +8231,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="85.5" customHeight="1">
+    <row r="51" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -8285,7 +8294,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="85.5" customHeight="1">
+    <row r="52" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -8328,7 +8337,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="220.5">
+    <row r="53" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -8393,7 +8402,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="85.5" customHeight="1">
+    <row r="54" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -8436,7 +8445,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="220.5">
+    <row r="55" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -8501,7 +8510,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="236.25">
+    <row r="56" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -8566,7 +8575,7 @@
       </c>
       <c r="W56" s="6"/>
     </row>
-    <row r="57" spans="1:23" ht="85.5" customHeight="1">
+    <row r="57" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -8607,7 +8616,7 @@
       <c r="V57" s="6"/>
       <c r="W57" s="6"/>
     </row>
-    <row r="58" spans="1:23" ht="85.5" customHeight="1">
+    <row r="58" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -8650,7 +8659,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="85.5" customHeight="1">
+    <row r="59" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -8691,7 +8700,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="85.5" customHeight="1">
+    <row r="60" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -8734,7 +8743,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="85.5" customHeight="1">
+    <row r="61" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -8775,7 +8784,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="85.5" customHeight="1">
+    <row r="62" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -8816,7 +8825,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="85.5" customHeight="1">
+    <row r="63" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -8859,7 +8868,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="85.5" customHeight="1">
+    <row r="64" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -8902,7 +8911,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="85.15" customHeight="1">
+    <row r="65" spans="1:23" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -8967,7 +8976,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="85.5" customHeight="1">
+    <row r="66" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -9010,7 +9019,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="85.5" customHeight="1">
+    <row r="67" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -9053,7 +9062,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="85.5" customHeight="1">
+    <row r="68" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -9096,7 +9105,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="85.5" customHeight="1">
+    <row r="69" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -9139,7 +9148,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="204.75">
+    <row r="70" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -9204,7 +9213,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="204.75">
+    <row r="71" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -9271,7 +9280,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="85.5" customHeight="1">
+    <row r="72" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -9314,7 +9323,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="204.75">
+    <row r="73" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -9377,7 +9386,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="252">
+    <row r="74" spans="1:23" ht="252" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -9442,7 +9451,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="252">
+    <row r="75" spans="1:23" ht="252" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>73</v>
       </c>
@@ -9507,7 +9516,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="141.75">
+    <row r="76" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>74</v>
       </c>
@@ -9568,7 +9577,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="189">
+    <row r="77" spans="1:23" ht="189" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>75</v>
       </c>
@@ -9633,7 +9642,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="126">
+    <row r="78" spans="1:23" ht="126" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>76</v>
       </c>
@@ -9698,7 +9707,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="85.5" customHeight="1">
+    <row r="79" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>77</v>
       </c>
@@ -9741,7 +9750,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="85.5" customHeight="1">
+    <row r="80" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>78</v>
       </c>
@@ -9782,7 +9791,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="236.25">
+    <row r="81" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>79</v>
       </c>
@@ -9847,7 +9856,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="85.5" customHeight="1">
+    <row r="82" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>80</v>
       </c>
@@ -9890,7 +9899,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="220.5">
+    <row r="83" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>81</v>
       </c>
@@ -9955,7 +9964,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="220.5">
+    <row r="84" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>81</v>
       </c>
@@ -10020,7 +10029,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="85.5" customHeight="1">
+    <row r="85" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>82</v>
       </c>
@@ -10059,7 +10068,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="85.5" customHeight="1">
+    <row r="86" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <v>83</v>
       </c>
@@ -10100,7 +10109,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="85.5" customHeight="1">
+    <row r="87" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>84</v>
       </c>
@@ -10143,7 +10152,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="204.75">
+    <row r="88" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>85</v>
       </c>
@@ -10202,7 +10211,7 @@
       <c r="V88" s="6"/>
       <c r="W88" s="6"/>
     </row>
-    <row r="89" spans="1:23" ht="85.5" customHeight="1">
+    <row r="89" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
         <v>86</v>
       </c>
@@ -10265,7 +10274,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="236.25">
+    <row r="90" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>87</v>
       </c>
@@ -10326,7 +10335,7 @@
       </c>
       <c r="W90" s="6"/>
     </row>
-    <row r="91" spans="1:23" ht="220.5">
+    <row r="91" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>88</v>
       </c>
@@ -10391,7 +10400,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="141.75">
+    <row r="92" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>89</v>
       </c>
@@ -10456,7 +10465,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="220.5">
+    <row r="93" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>90</v>
       </c>
@@ -10521,7 +10530,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="85.5" customHeight="1">
+    <row r="94" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>91</v>
       </c>
@@ -10556,7 +10565,7 @@
       <c r="V94" s="6"/>
       <c r="W94" s="6"/>
     </row>
-    <row r="95" spans="1:23" ht="85.5" customHeight="1">
+    <row r="95" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>92</v>
       </c>
@@ -10597,7 +10606,7 @@
       <c r="V95" s="6"/>
       <c r="W95" s="6"/>
     </row>
-    <row r="96" spans="1:23" ht="78.75">
+    <row r="96" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>93</v>
       </c>
@@ -10660,7 +10669,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="85.5" customHeight="1">
+    <row r="97" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
         <v>94</v>
       </c>
@@ -10699,7 +10708,7 @@
       <c r="V97" s="6"/>
       <c r="W97" s="6"/>
     </row>
-    <row r="98" spans="1:23" ht="220.5">
+    <row r="98" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>95</v>
       </c>
@@ -10762,7 +10771,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="141.75">
+    <row r="99" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>96</v>
       </c>
@@ -10825,7 +10834,7 @@
       </c>
       <c r="W99" s="6"/>
     </row>
-    <row r="100" spans="1:23" ht="85.5" customHeight="1">
+    <row r="100" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
         <v>97</v>
       </c>
@@ -10862,7 +10871,7 @@
       <c r="V100" s="6"/>
       <c r="W100" s="6"/>
     </row>
-    <row r="101" spans="1:23" ht="85.5" customHeight="1">
+    <row r="101" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>98</v>
       </c>
@@ -10899,7 +10908,7 @@
       <c r="V101" s="6"/>
       <c r="W101" s="6"/>
     </row>
-    <row r="102" spans="1:23" ht="204.75">
+    <row r="102" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>99</v>
       </c>
@@ -10962,7 +10971,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="85.5" customHeight="1">
+    <row r="103" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>100</v>
       </c>
@@ -11005,7 +11014,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="126">
+    <row r="104" spans="1:23" ht="126" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>101</v>
       </c>
@@ -11070,7 +11079,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="94.5">
+    <row r="105" spans="1:23" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>102</v>
       </c>
@@ -11135,7 +11144,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="85.5" customHeight="1">
+    <row r="106" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>103</v>
       </c>
@@ -11172,7 +11181,7 @@
       <c r="V106" s="6"/>
       <c r="W106" s="6"/>
     </row>
-    <row r="107" spans="1:23" ht="236.25">
+    <row r="107" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A107" s="6">
         <v>104</v>
       </c>
@@ -11235,7 +11244,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="220.5">
+    <row r="108" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
         <v>105</v>
       </c>
@@ -11296,7 +11305,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="141.75">
+    <row r="109" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>106</v>
       </c>
@@ -11357,7 +11366,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="141.75">
+    <row r="110" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
         <v>106</v>
       </c>
@@ -11418,7 +11427,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="204.75">
+    <row r="111" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
         <v>107</v>
       </c>
@@ -11481,7 +11490,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="204.75">
+    <row r="112" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
         <v>107</v>
       </c>
@@ -11544,7 +11553,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="85.5" customHeight="1">
+    <row r="113" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6">
         <v>108</v>
       </c>
@@ -11583,7 +11592,7 @@
       <c r="V113" s="6"/>
       <c r="W113" s="6"/>
     </row>
-    <row r="114" spans="1:23" ht="85.5" customHeight="1">
+    <row r="114" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>109</v>
       </c>
@@ -11622,7 +11631,7 @@
       <c r="V114" s="6"/>
       <c r="W114" s="6"/>
     </row>
-    <row r="115" spans="1:23" ht="236.25">
+    <row r="115" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>110</v>
       </c>
@@ -11687,7 +11696,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="85.5" customHeight="1">
+    <row r="116" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>111</v>
       </c>
@@ -11726,7 +11735,7 @@
       <c r="V116" s="6"/>
       <c r="W116" s="6"/>
     </row>
-    <row r="117" spans="1:23" ht="85.5" customHeight="1">
+    <row r="117" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6">
         <v>112</v>
       </c>
@@ -11763,7 +11772,7 @@
       <c r="V117" s="6"/>
       <c r="W117" s="6"/>
     </row>
-    <row r="118" spans="1:23" ht="236.25">
+    <row r="118" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A118" s="6">
         <v>113</v>
       </c>
@@ -11824,7 +11833,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="204.75">
+    <row r="119" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A119" s="6">
         <v>114</v>
       </c>
@@ -11885,7 +11894,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="85.5" customHeight="1">
+    <row r="120" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>115</v>
       </c>
@@ -11926,7 +11935,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="85.5" customHeight="1">
+    <row r="121" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6">
         <v>116</v>
       </c>
@@ -11965,7 +11974,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="141.75">
+    <row r="122" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A122" s="6">
         <v>117</v>
       </c>
@@ -12024,7 +12033,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="85.5" customHeight="1">
+    <row r="123" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6">
         <v>118</v>
       </c>
@@ -12067,7 +12076,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="85.5" customHeight="1">
+    <row r="124" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6">
         <v>119</v>
       </c>
@@ -12110,7 +12119,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="204.75">
+    <row r="125" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A125" s="6">
         <v>120</v>
       </c>
@@ -12173,7 +12182,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="204.75">
+    <row r="126" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A126" s="6">
         <v>121</v>
       </c>
@@ -12234,7 +12243,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="85.5" customHeight="1">
+    <row r="127" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6">
         <v>121</v>
       </c>
@@ -12275,7 +12284,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="85.5" customHeight="1">
+    <row r="128" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6">
         <v>122</v>
       </c>
@@ -12312,7 +12321,7 @@
       <c r="V128" s="6"/>
       <c r="W128" s="6"/>
     </row>
-    <row r="129" spans="1:23" ht="85.5" customHeight="1">
+    <row r="129" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6">
         <v>123</v>
       </c>
@@ -12355,7 +12364,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="85.5" customHeight="1">
+    <row r="130" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6">
         <v>124</v>
       </c>
@@ -12390,7 +12399,7 @@
       <c r="V130" s="6"/>
       <c r="W130" s="6"/>
     </row>
-    <row r="131" spans="1:23" ht="220.5">
+    <row r="131" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A131" s="6">
         <v>125</v>
       </c>
@@ -12453,7 +12462,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="85.5" customHeight="1">
+    <row r="132" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6">
         <v>126</v>
       </c>
@@ -12496,7 +12505,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="85.5" customHeight="1">
+    <row r="133" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6">
         <v>126</v>
       </c>
@@ -12539,7 +12548,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="85.5" customHeight="1">
+    <row r="134" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6">
         <v>127</v>
       </c>
@@ -12600,7 +12609,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="220.5">
+    <row r="135" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A135" s="6">
         <v>128</v>
       </c>
@@ -12661,7 +12670,7 @@
       </c>
       <c r="W135" s="6"/>
     </row>
-    <row r="136" spans="1:23" ht="236.25">
+    <row r="136" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A136" s="6">
         <v>129</v>
       </c>
@@ -12722,7 +12731,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="85.5" customHeight="1">
+    <row r="137" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6">
         <v>130</v>
       </c>
@@ -12759,7 +12768,7 @@
       <c r="V137" s="7"/>
       <c r="W137" s="6"/>
     </row>
-    <row r="138" spans="1:23" ht="252">
+    <row r="138" spans="1:23" ht="252" x14ac:dyDescent="0.25">
       <c r="A138" s="6">
         <v>131</v>
       </c>
@@ -12824,7 +12833,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="85.5" customHeight="1">
+    <row r="139" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6">
         <v>132</v>
       </c>
@@ -12861,7 +12870,7 @@
       <c r="V139" s="6"/>
       <c r="W139" s="6"/>
     </row>
-    <row r="140" spans="1:23" ht="236.25">
+    <row r="140" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A140" s="6">
         <v>133</v>
       </c>
@@ -12924,7 +12933,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="157.5">
+    <row r="141" spans="1:23" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A141" s="6">
         <v>134</v>
       </c>
@@ -12987,7 +12996,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="126">
+    <row r="142" spans="1:23" ht="126" x14ac:dyDescent="0.25">
       <c r="A142" s="6">
         <v>135</v>
       </c>
@@ -13050,7 +13059,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="85.5" customHeight="1">
+    <row r="143" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6">
         <v>136</v>
       </c>
@@ -13095,7 +13104,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="85.5" customHeight="1">
+    <row r="144" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6">
         <v>137</v>
       </c>
@@ -13136,7 +13145,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="85.5" customHeight="1">
+    <row r="145" spans="1:23" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6">
         <v>138</v>
       </c>
@@ -13179,7 +13188,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="252">
+    <row r="146" spans="1:23" ht="252" x14ac:dyDescent="0.25">
       <c r="A146" s="6">
         <v>139</v>
       </c>
@@ -13242,7 +13251,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="252">
+    <row r="147" spans="1:23" ht="252" x14ac:dyDescent="0.25">
       <c r="A147" s="6">
         <v>139</v>
       </c>
@@ -13305,7 +13314,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="236.25">
+    <row r="148" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A148" s="6">
         <v>140</v>
       </c>
@@ -13364,7 +13373,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="149" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6">
         <v>141</v>
       </c>
@@ -13399,7 +13408,7 @@
       <c r="V149" s="6"/>
       <c r="W149" s="6"/>
     </row>
-    <row r="150" spans="1:23" ht="94.5">
+    <row r="150" spans="1:23" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A150" s="6">
         <v>142</v>
       </c>
@@ -13462,7 +13471,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="151" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6">
         <v>143</v>
       </c>
@@ -13505,7 +13514,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="220.5">
+    <row r="152" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A152" s="6">
         <v>144</v>
       </c>
@@ -13566,7 +13575,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="126">
+    <row r="153" spans="1:23" ht="126" x14ac:dyDescent="0.25">
       <c r="A153" s="6">
         <v>145</v>
       </c>
@@ -13629,7 +13638,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="154" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>146</v>
       </c>
@@ -13672,7 +13681,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="155" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6">
         <v>147</v>
       </c>
@@ -13717,7 +13726,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="156" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="6">
         <v>147</v>
       </c>
@@ -13762,7 +13771,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="157" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6">
         <v>148</v>
       </c>
@@ -13805,7 +13814,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="158" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6">
         <v>149</v>
       </c>
@@ -13848,7 +13857,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="78.75">
+    <row r="159" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A159" s="6">
         <v>150</v>
       </c>
@@ -13909,7 +13918,7 @@
       </c>
       <c r="W159" s="6"/>
     </row>
-    <row r="160" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="160" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6">
         <v>151</v>
       </c>
@@ -13952,7 +13961,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="110.25">
+    <row r="161" spans="1:23" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A161" s="6">
         <v>152</v>
       </c>
@@ -14015,7 +14024,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="110.25">
+    <row r="162" spans="1:23" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A162" s="6">
         <v>152</v>
       </c>
@@ -14078,7 +14087,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="236.25">
+    <row r="163" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A163" s="6">
         <v>153</v>
       </c>
@@ -14139,7 +14148,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="189">
+    <row r="164" spans="1:23" ht="189" x14ac:dyDescent="0.25">
       <c r="A164" s="6">
         <v>154</v>
       </c>
@@ -14200,7 +14209,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="165" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="6">
         <v>155</v>
       </c>
@@ -14239,7 +14248,7 @@
       <c r="V165" s="6"/>
       <c r="W165" s="6"/>
     </row>
-    <row r="166" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="166" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="6">
         <v>156</v>
       </c>
@@ -14280,7 +14289,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="167" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="6">
         <v>157</v>
       </c>
@@ -14319,7 +14328,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="168" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="6">
         <v>158</v>
       </c>
@@ -14362,7 +14371,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="169" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="6">
         <v>159</v>
       </c>
@@ -14403,7 +14412,7 @@
       </c>
       <c r="W169" s="6"/>
     </row>
-    <row r="170" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="170" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6">
         <v>160</v>
       </c>
@@ -14446,7 +14455,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="171" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="6">
         <v>161</v>
       </c>
@@ -14489,7 +14498,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="172" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="6">
         <v>162</v>
       </c>
@@ -14530,7 +14539,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="173" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="6">
         <v>163</v>
       </c>
@@ -14571,7 +14580,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="174" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="6">
         <v>164</v>
       </c>
@@ -14612,7 +14621,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="175" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="6">
         <v>165</v>
       </c>
@@ -14653,7 +14662,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="157.5">
+    <row r="176" spans="1:23" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A176" s="6">
         <v>166</v>
       </c>
@@ -14716,7 +14725,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="177" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6">
         <v>167</v>
       </c>
@@ -14759,7 +14768,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="178" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6">
         <v>168</v>
       </c>
@@ -14800,7 +14809,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="78.75">
+    <row r="179" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A179" s="6">
         <v>169</v>
       </c>
@@ -14865,7 +14874,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="180" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6">
         <v>170</v>
       </c>
@@ -14908,7 +14917,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="181" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6">
         <v>171</v>
       </c>
@@ -14951,7 +14960,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="182" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="6">
         <v>172</v>
       </c>
@@ -14992,7 +15001,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="183" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="6">
         <v>173</v>
       </c>
@@ -15031,7 +15040,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="184" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="6">
         <v>174</v>
       </c>
@@ -15070,7 +15079,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="78.75">
+    <row r="185" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A185" s="6">
         <v>175</v>
       </c>
@@ -15133,7 +15142,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="186" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="6">
         <v>176</v>
       </c>
@@ -15172,7 +15181,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="187" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="6">
         <v>177</v>
       </c>
@@ -15233,7 +15242,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="188" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="6">
         <v>178</v>
       </c>
@@ -15272,7 +15281,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="189" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="6">
         <v>179</v>
       </c>
@@ -15337,7 +15346,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="190" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="6">
         <v>180</v>
       </c>
@@ -15380,7 +15389,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="252">
+    <row r="191" spans="1:23" ht="252" x14ac:dyDescent="0.25">
       <c r="A191" s="6">
         <v>181</v>
       </c>
@@ -15443,7 +15452,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="192" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="6">
         <v>182</v>
       </c>
@@ -15484,7 +15493,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="236.25">
+    <row r="193" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A193" s="6">
         <v>183</v>
       </c>
@@ -15545,7 +15554,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="194" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="6">
         <v>184</v>
       </c>
@@ -15588,7 +15597,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="195" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="195" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="6">
         <v>185</v>
       </c>
@@ -15631,7 +15640,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="196" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="196" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="6">
         <v>186</v>
       </c>
@@ -15674,7 +15683,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="197" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="197" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="6">
         <v>187</v>
       </c>
@@ -15715,7 +15724,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="198" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="198" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="6">
         <v>188</v>
       </c>
@@ -15774,7 +15783,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="199" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="6">
         <v>189</v>
       </c>
@@ -15817,7 +15826,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="200" spans="1:23" ht="173.25">
+    <row r="200" spans="1:23" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A200" s="6">
         <v>190</v>
       </c>
@@ -15880,7 +15889,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="201" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="201" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="6">
         <v>191</v>
       </c>
@@ -15921,7 +15930,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="202" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="202" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="6">
         <v>192</v>
       </c>
@@ -15960,7 +15969,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="203" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="203" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="6">
         <v>193</v>
       </c>
@@ -15999,7 +16008,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="204" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="204" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="6">
         <v>194</v>
       </c>
@@ -16040,7 +16049,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="205" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="205" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="6">
         <v>195</v>
       </c>
@@ -16081,7 +16090,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="206" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="206" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="6">
         <v>196</v>
       </c>
@@ -16118,7 +16127,7 @@
       <c r="V206" s="6"/>
       <c r="W206" s="6"/>
     </row>
-    <row r="207" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="207" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="6">
         <v>197</v>
       </c>
@@ -16159,7 +16168,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="208" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="208" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="6">
         <v>198</v>
       </c>
@@ -16200,7 +16209,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="209" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="209" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="6">
         <v>199</v>
       </c>
@@ -16243,7 +16252,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="210" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="210" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="6">
         <v>200</v>
       </c>
@@ -16284,7 +16293,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="211" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="211" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="6">
         <v>201</v>
       </c>
@@ -16325,7 +16334,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="212" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="212" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="6">
         <v>202</v>
       </c>
@@ -16366,7 +16375,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="213" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="213" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="6">
         <v>203</v>
       </c>
@@ -16409,7 +16418,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="214" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="214" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="6">
         <v>204</v>
       </c>
@@ -16450,7 +16459,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="215" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="215" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="6">
         <v>205</v>
       </c>
@@ -16491,7 +16500,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="216" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="216" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="6">
         <v>206</v>
       </c>
@@ -16532,7 +16541,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="217" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="217" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="6">
         <v>207</v>
       </c>
@@ -16569,7 +16578,7 @@
       <c r="V217" s="6"/>
       <c r="W217" s="6"/>
     </row>
-    <row r="218" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="218" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="6">
         <v>208</v>
       </c>
@@ -16604,7 +16613,7 @@
       <c r="V218" s="6"/>
       <c r="W218" s="6"/>
     </row>
-    <row r="219" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="219" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="6">
         <v>209</v>
       </c>
@@ -16645,7 +16654,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="220" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="220" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="6">
         <v>210</v>
       </c>
@@ -16686,7 +16695,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="221" spans="1:23" ht="73.900000000000006" customHeight="1">
+    <row r="221" spans="1:23" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="6">
         <v>211</v>
       </c>
@@ -16723,7 +16732,7 @@
       <c r="V221" s="7"/>
       <c r="W221" s="7"/>
     </row>
-    <row r="222" spans="1:23" ht="88.5" customHeight="1">
+    <row r="222" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="6">
         <v>212</v>
       </c>
@@ -16764,7 +16773,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="223" spans="1:23" ht="88.5" customHeight="1">
+    <row r="223" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="6">
         <v>213</v>
       </c>
@@ -16805,7 +16814,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="224" spans="1:23" ht="88.5" customHeight="1">
+    <row r="224" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="6">
         <v>214</v>
       </c>
@@ -16846,7 +16855,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="225" spans="1:23" ht="88.5" customHeight="1">
+    <row r="225" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="6">
         <v>215</v>
       </c>
@@ -16885,7 +16894,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="226" spans="1:23" ht="88.5" customHeight="1">
+    <row r="226" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="6">
         <v>216</v>
       </c>
@@ -16926,7 +16935,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="227" spans="1:23" ht="88.5" customHeight="1">
+    <row r="227" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="6">
         <v>217</v>
       </c>
@@ -16965,7 +16974,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="228" spans="1:23" ht="88.5" customHeight="1">
+    <row r="228" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="6">
         <v>218</v>
       </c>
@@ -17006,7 +17015,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="229" spans="1:23" ht="88.5" customHeight="1">
+    <row r="229" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="6">
         <v>219</v>
       </c>
@@ -17045,7 +17054,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="230" spans="1:23" ht="88.5" customHeight="1">
+    <row r="230" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="6">
         <v>220</v>
       </c>
@@ -17084,7 +17093,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="231" spans="1:23" ht="88.5" customHeight="1">
+    <row r="231" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="6">
         <v>221</v>
       </c>
@@ -17125,7 +17134,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="232" spans="1:23" ht="88.5" customHeight="1">
+    <row r="232" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="6">
         <v>222</v>
       </c>
@@ -17162,7 +17171,7 @@
       <c r="V232" s="7"/>
       <c r="W232" s="7"/>
     </row>
-    <row r="233" spans="1:23" ht="88.5" customHeight="1">
+    <row r="233" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="6">
         <v>223</v>
       </c>
@@ -17203,7 +17212,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="234" spans="1:23" ht="88.5" customHeight="1">
+    <row r="234" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="6">
         <v>224</v>
       </c>
@@ -17244,7 +17253,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="235" spans="1:23" ht="88.5" customHeight="1">
+    <row r="235" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="6">
         <v>225</v>
       </c>
@@ -17283,7 +17292,7 @@
       <c r="V235" s="7"/>
       <c r="W235" s="7"/>
     </row>
-    <row r="236" spans="1:23" ht="88.5" customHeight="1">
+    <row r="236" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="6">
         <v>226</v>
       </c>
@@ -17324,7 +17333,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="237" spans="1:23" ht="88.5" customHeight="1">
+    <row r="237" spans="1:23" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="6">
         <v>227</v>
       </c>
@@ -17363,7 +17372,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="238" spans="1:23" ht="73.5" customHeight="1">
+    <row r="238" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="6">
         <v>228</v>
       </c>
@@ -17404,7 +17413,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="239" spans="1:23" ht="73.5" customHeight="1">
+    <row r="239" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="6">
         <v>229</v>
       </c>
@@ -17445,7 +17454,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="240" spans="1:23" ht="73.5" customHeight="1">
+    <row r="240" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="6">
         <v>230</v>
       </c>
@@ -17486,7 +17495,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="241" spans="1:23" ht="73.5" customHeight="1">
+    <row r="241" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="6">
         <v>231</v>
       </c>
@@ -17527,7 +17536,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="242" spans="1:23" ht="73.5" customHeight="1">
+    <row r="242" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="6">
         <v>232</v>
       </c>
@@ -17568,7 +17577,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="243" spans="1:23" ht="73.5" customHeight="1">
+    <row r="243" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="6">
         <v>233</v>
       </c>
@@ -17609,7 +17618,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="244" spans="1:23" ht="73.5" customHeight="1">
+    <row r="244" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="6">
         <v>234</v>
       </c>
@@ -17650,7 +17659,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="245" spans="1:23" ht="73.5" customHeight="1">
+    <row r="245" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="6">
         <v>235</v>
       </c>
@@ -17691,7 +17700,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="246" spans="1:23" ht="73.5" customHeight="1">
+    <row r="246" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="6">
         <v>236</v>
       </c>
@@ -17730,7 +17739,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="247" spans="1:23" ht="236.25">
+    <row r="247" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A247" s="6">
         <v>237</v>
       </c>
@@ -17791,7 +17800,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="248" spans="1:23" ht="73.5" customHeight="1">
+    <row r="248" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="6">
         <v>238</v>
       </c>
@@ -17834,7 +17843,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="249" spans="1:23" ht="73.5" customHeight="1">
+    <row r="249" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="6">
         <v>238</v>
       </c>
@@ -17877,7 +17886,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="250" spans="1:23" ht="73.5" customHeight="1">
+    <row r="250" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="6">
         <v>239</v>
       </c>
@@ -17918,7 +17927,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="251" spans="1:23" ht="73.5" customHeight="1">
+    <row r="251" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="6">
         <v>240</v>
       </c>
@@ -17955,7 +17964,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="252" spans="1:23" ht="157.5">
+    <row r="252" spans="1:23" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A252" s="6">
         <v>241</v>
       </c>
@@ -18020,7 +18029,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="253" spans="1:23" ht="141.75">
+    <row r="253" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A253" s="6">
         <v>242</v>
       </c>
@@ -18079,7 +18088,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="254" spans="1:23" ht="73.5" customHeight="1">
+    <row r="254" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="6">
         <v>243</v>
       </c>
@@ -18116,7 +18125,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="255" spans="1:23" ht="73.5" customHeight="1">
+    <row r="255" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="6">
         <v>244</v>
       </c>
@@ -18153,7 +18162,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="256" spans="1:23" ht="73.5" customHeight="1">
+    <row r="256" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="6">
         <v>245</v>
       </c>
@@ -18194,7 +18203,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="257" spans="1:23" ht="220.5">
+    <row r="257" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A257" s="6">
         <v>246</v>
       </c>
@@ -18255,7 +18264,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="258" spans="1:23" ht="73.5" customHeight="1">
+    <row r="258" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="6">
         <v>247</v>
       </c>
@@ -18294,7 +18303,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="259" spans="1:23" ht="73.5" customHeight="1">
+    <row r="259" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="6">
         <v>248</v>
       </c>
@@ -18335,7 +18344,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="260" spans="1:23" ht="73.5" customHeight="1">
+    <row r="260" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="6">
         <v>249</v>
       </c>
@@ -18376,7 +18385,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="261" spans="1:23" ht="189">
+    <row r="261" spans="1:23" ht="189" x14ac:dyDescent="0.25">
       <c r="A261" s="6">
         <v>250</v>
       </c>
@@ -18437,7 +18446,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="262" spans="1:23" ht="73.5" customHeight="1">
+    <row r="262" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="6">
         <v>251</v>
       </c>
@@ -18476,7 +18485,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="263" spans="1:23" ht="236.25">
+    <row r="263" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A263" s="6">
         <v>252</v>
       </c>
@@ -18537,7 +18546,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="264" spans="1:23" ht="73.5" customHeight="1">
+    <row r="264" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="6">
         <v>253</v>
       </c>
@@ -18574,7 +18583,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="265" spans="1:23" ht="73.5" customHeight="1">
+    <row r="265" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="6">
         <v>254</v>
       </c>
@@ -18613,7 +18622,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="266" spans="1:23" ht="73.5" customHeight="1">
+    <row r="266" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="6">
         <v>255</v>
       </c>
@@ -18650,7 +18659,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="267" spans="1:23" ht="189">
+    <row r="267" spans="1:23" ht="189" x14ac:dyDescent="0.25">
       <c r="A267" s="6">
         <v>256</v>
       </c>
@@ -18713,7 +18722,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="268" spans="1:23" ht="73.5" customHeight="1">
+    <row r="268" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="6">
         <v>257</v>
       </c>
@@ -18758,7 +18767,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="269" spans="1:23" ht="73.5" customHeight="1">
+    <row r="269" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="6">
         <v>258</v>
       </c>
@@ -18799,7 +18808,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="270" spans="1:23" ht="73.5" customHeight="1">
+    <row r="270" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="6">
         <v>259</v>
       </c>
@@ -18842,7 +18851,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="271" spans="1:23" ht="220.5">
+    <row r="271" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A271" s="6">
         <v>260</v>
       </c>
@@ -18905,7 +18914,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="272" spans="1:23" ht="73.5" customHeight="1">
+    <row r="272" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="6">
         <v>261</v>
       </c>
@@ -18946,7 +18955,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="273" spans="1:23" ht="73.5" customHeight="1">
+    <row r="273" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="6">
         <v>262</v>
       </c>
@@ -18987,7 +18996,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="274" spans="1:23" ht="73.5" customHeight="1">
+    <row r="274" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="6">
         <v>263</v>
       </c>
@@ -19028,7 +19037,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="275" spans="1:23" ht="157.5">
+    <row r="275" spans="1:23" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A275" s="6">
         <v>264</v>
       </c>
@@ -19091,7 +19100,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="276" spans="1:23" ht="73.5" customHeight="1">
+    <row r="276" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="6">
         <v>265</v>
       </c>
@@ -19134,7 +19143,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="277" spans="1:23" ht="73.5" customHeight="1">
+    <row r="277" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="6">
         <v>265</v>
       </c>
@@ -19177,7 +19186,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="278" spans="1:23" ht="73.5" customHeight="1">
+    <row r="278" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="6">
         <v>266</v>
       </c>
@@ -19216,7 +19225,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="279" spans="1:23" ht="236.25">
+    <row r="279" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A279" s="6">
         <v>267</v>
       </c>
@@ -19281,7 +19290,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="280" spans="1:23" ht="236.25">
+    <row r="280" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A280" s="6">
         <v>268</v>
       </c>
@@ -19344,7 +19353,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="281" spans="1:23" ht="73.5" customHeight="1">
+    <row r="281" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="6">
         <v>269</v>
       </c>
@@ -19381,7 +19390,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="282" spans="1:23" ht="73.5" customHeight="1">
+    <row r="282" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="6">
         <v>270</v>
       </c>
@@ -19420,7 +19429,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="283" spans="1:23" ht="126">
+    <row r="283" spans="1:23" ht="126" x14ac:dyDescent="0.25">
       <c r="A283" s="6">
         <v>271</v>
       </c>
@@ -19483,7 +19492,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="284" spans="1:23" ht="73.5" customHeight="1">
+    <row r="284" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="6">
         <v>272</v>
       </c>
@@ -19526,7 +19535,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="285" spans="1:23" ht="236.25">
+    <row r="285" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A285" s="6">
         <v>273</v>
       </c>
@@ -19591,7 +19600,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="286" spans="1:23" ht="141.75">
+    <row r="286" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A286" s="6">
         <v>274</v>
       </c>
@@ -19654,7 +19663,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="287" spans="1:23" ht="73.5" customHeight="1">
+    <row r="287" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="6">
         <v>275</v>
       </c>
@@ -19697,7 +19706,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="288" spans="1:23" ht="73.5" customHeight="1">
+    <row r="288" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="6">
         <v>276</v>
       </c>
@@ -19734,7 +19743,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="289" spans="1:24" ht="157.5">
+    <row r="289" spans="1:24" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A289" s="6">
         <v>277</v>
       </c>
@@ -19797,7 +19806,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="290" spans="1:24" ht="73.5" customHeight="1">
+    <row r="290" spans="1:24" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="6">
         <v>278</v>
       </c>
@@ -19840,7 +19849,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="291" spans="1:24" ht="73.5" customHeight="1">
+    <row r="291" spans="1:24" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="6">
         <v>279</v>
       </c>
@@ -19883,7 +19892,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="292" spans="1:24" ht="73.5" customHeight="1">
+    <row r="292" spans="1:24" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="6">
         <v>280</v>
       </c>
@@ -19926,7 +19935,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="293" spans="1:24" ht="73.5" customHeight="1">
+    <row r="293" spans="1:24" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="6">
         <v>281</v>
       </c>
@@ -19969,7 +19978,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="294" spans="1:24" ht="73.5" customHeight="1">
+    <row r="294" spans="1:24" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="6">
         <v>282</v>
       </c>
@@ -20008,7 +20017,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="295" spans="1:24" ht="236.25">
+    <row r="295" spans="1:24" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A295" s="6">
         <v>283</v>
       </c>
@@ -20069,7 +20078,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="296" spans="1:24" ht="126">
+    <row r="296" spans="1:24" ht="126" x14ac:dyDescent="0.25">
       <c r="A296" s="6">
         <v>284</v>
       </c>
@@ -20130,7 +20139,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="297" spans="1:24" ht="220.5">
+    <row r="297" spans="1:24" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A297" s="6">
         <v>285</v>
       </c>
@@ -20191,7 +20200,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="298" spans="1:24" ht="157.5">
+    <row r="298" spans="1:24" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A298" s="6">
         <v>286</v>
       </c>
@@ -20252,7 +20261,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="299" spans="1:24" s="3" customFormat="1" ht="73.5" customHeight="1">
+    <row r="299" spans="1:24" s="3" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="6">
         <v>287</v>
       </c>
@@ -20294,7 +20303,7 @@
       </c>
       <c r="X299" s="5"/>
     </row>
-    <row r="300" spans="1:24" ht="236.25">
+    <row r="300" spans="1:24" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A300" s="6">
         <v>288</v>
       </c>
@@ -20357,7 +20366,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="301" spans="1:24" ht="73.5" customHeight="1">
+    <row r="301" spans="1:24" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="6">
         <v>289</v>
       </c>
@@ -20400,7 +20409,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="302" spans="1:24" ht="236.25">
+    <row r="302" spans="1:24" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A302" s="6">
         <v>290</v>
       </c>
@@ -20465,7 +20474,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="303" spans="1:24" ht="189">
+    <row r="303" spans="1:24" ht="189" x14ac:dyDescent="0.25">
       <c r="A303" s="6">
         <v>291</v>
       </c>
@@ -20530,7 +20539,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="304" spans="1:24" ht="73.5" customHeight="1">
+    <row r="304" spans="1:24" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="6">
         <v>292</v>
       </c>
@@ -20573,7 +20582,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="305" spans="1:23" ht="73.5" customHeight="1">
+    <row r="305" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="6">
         <v>293</v>
       </c>
@@ -20616,7 +20625,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="306" spans="1:23" ht="220.5">
+    <row r="306" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A306" s="6">
         <v>294</v>
       </c>
@@ -20681,7 +20690,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="307" spans="1:23" ht="236.25">
+    <row r="307" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A307" s="6">
         <v>295</v>
       </c>
@@ -20744,7 +20753,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="308" spans="1:23" ht="220.5">
+    <row r="308" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A308" s="6">
         <v>296</v>
       </c>
@@ -20811,7 +20820,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="309" spans="1:23" ht="73.5" customHeight="1">
+    <row r="309" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="6">
         <v>297</v>
       </c>
@@ -20850,7 +20859,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="310" spans="1:23" ht="73.5" customHeight="1">
+    <row r="310" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="6">
         <v>298</v>
       </c>
@@ -20893,7 +20902,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="311" spans="1:23" ht="220.5">
+    <row r="311" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A311" s="6">
         <v>299</v>
       </c>
@@ -20956,7 +20965,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="312" spans="1:23" ht="73.5" customHeight="1">
+    <row r="312" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="6">
         <v>300</v>
       </c>
@@ -20999,7 +21008,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="313" spans="1:23" ht="73.5" customHeight="1">
+    <row r="313" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="6">
         <v>301</v>
       </c>
@@ -21040,7 +21049,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="314" spans="1:23" ht="204.75">
+    <row r="314" spans="1:23" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A314" s="6">
         <v>302</v>
       </c>
@@ -21103,7 +21112,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="315" spans="1:23" ht="173.25">
+    <row r="315" spans="1:23" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A315" s="6">
         <v>303</v>
       </c>
@@ -21164,7 +21173,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="316" spans="1:23" ht="73.5" customHeight="1">
+    <row r="316" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="6">
         <v>304</v>
       </c>
@@ -21207,7 +21216,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="317" spans="1:23" ht="73.5" customHeight="1">
+    <row r="317" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="6">
         <v>305</v>
       </c>
@@ -21248,7 +21257,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="318" spans="1:23" ht="73.5" customHeight="1">
+    <row r="318" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="6">
         <v>306</v>
       </c>
@@ -21291,7 +21300,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="319" spans="1:23" ht="173.25">
+    <row r="319" spans="1:23" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A319" s="6">
         <v>307</v>
       </c>
@@ -21352,7 +21361,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="320" spans="1:23" ht="236.25">
+    <row r="320" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A320" s="6">
         <v>308</v>
       </c>
@@ -21413,7 +21422,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="321" spans="1:23" ht="73.5" customHeight="1">
+    <row r="321" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="6">
         <v>309</v>
       </c>
@@ -21452,7 +21461,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="322" spans="1:23" ht="73.5" customHeight="1">
+    <row r="322" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="6">
         <v>310</v>
       </c>
@@ -21495,7 +21504,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="323" spans="1:23" ht="110.25">
+    <row r="323" spans="1:23" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A323" s="6">
         <v>311</v>
       </c>
@@ -21558,7 +21567,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="324" spans="1:23" ht="220.5">
+    <row r="324" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A324" s="6">
         <v>312</v>
       </c>
@@ -21621,7 +21630,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="325" spans="1:23" ht="73.5" customHeight="1">
+    <row r="325" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="6">
         <v>313</v>
       </c>
@@ -21660,7 +21669,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="326" spans="1:23" ht="73.5" customHeight="1">
+    <row r="326" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="6">
         <v>314</v>
       </c>
@@ -21703,7 +21712,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="327" spans="1:23" ht="73.5" customHeight="1">
+    <row r="327" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="6">
         <v>315</v>
       </c>
@@ -21744,7 +21753,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="328" spans="1:23" ht="173.25">
+    <row r="328" spans="1:23" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A328" s="6">
         <v>316</v>
       </c>
@@ -21805,7 +21814,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="329" spans="1:23" ht="73.5" customHeight="1">
+    <row r="329" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="6">
         <v>317</v>
       </c>
@@ -21848,7 +21857,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="330" spans="1:23" ht="73.5" customHeight="1">
+    <row r="330" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="6">
         <v>318</v>
       </c>
@@ -21889,7 +21898,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="331" spans="1:23" ht="73.5" customHeight="1">
+    <row r="331" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="6">
         <v>319</v>
       </c>
@@ -21930,7 +21939,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="332" spans="1:23" ht="141.75">
+    <row r="332" spans="1:23" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A332" s="6">
         <v>320</v>
       </c>
@@ -21989,7 +21998,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="333" spans="1:23" ht="236.25">
+    <row r="333" spans="1:23" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A333" s="6">
         <v>321</v>
       </c>
@@ -22048,7 +22057,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="334" spans="1:23" ht="73.5" customHeight="1">
+    <row r="334" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="6">
         <v>322</v>
       </c>
@@ -22089,7 +22098,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="335" spans="1:23" ht="73.5" customHeight="1">
+    <row r="335" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="6">
         <v>323</v>
       </c>
@@ -22128,7 +22137,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="336" spans="1:23" ht="73.5" customHeight="1">
+    <row r="336" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="6">
         <v>324</v>
       </c>
@@ -22169,7 +22178,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="337" spans="1:23" ht="73.5" customHeight="1">
+    <row r="337" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="6">
         <v>325</v>
       </c>
@@ -22210,7 +22219,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="338" spans="1:23" ht="73.5" customHeight="1">
+    <row r="338" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="6">
         <v>326</v>
       </c>
@@ -22251,7 +22260,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="339" spans="1:23" ht="73.5" customHeight="1">
+    <row r="339" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="6">
         <v>327</v>
       </c>
@@ -22292,7 +22301,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="340" spans="1:23" ht="73.5" customHeight="1">
+    <row r="340" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="6">
         <v>328</v>
       </c>
@@ -22333,7 +22342,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="341" spans="1:23" ht="73.5" customHeight="1">
+    <row r="341" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="6">
         <v>329</v>
       </c>
@@ -22374,7 +22383,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="342" spans="1:23" ht="220.5">
+    <row r="342" spans="1:23" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A342" s="6">
         <v>330</v>
       </c>
@@ -22431,7 +22440,7 @@
       </c>
       <c r="W342" s="6"/>
     </row>
-    <row r="343" spans="1:23" ht="73.5" customHeight="1">
+    <row r="343" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="6">
         <v>331</v>
       </c>
@@ -22470,7 +22479,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="344" spans="1:23" ht="73.5" customHeight="1">
+    <row r="344" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="6">
         <v>332</v>
       </c>
@@ -22509,7 +22518,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="345" spans="1:23" ht="189">
+    <row r="345" spans="1:23" ht="189" x14ac:dyDescent="0.25">
       <c r="A345" s="6">
         <v>333</v>
       </c>
@@ -22566,7 +22575,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="346" spans="1:23" ht="73.5" customHeight="1">
+    <row r="346" spans="1:23" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="6">
         <v>334</v>
       </c>
@@ -22607,7 +22616,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="347" spans="1:23" ht="73.150000000000006" customHeight="1">
+    <row r="347" spans="1:23" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="6">
         <v>335</v>
       </c>
@@ -22646,7 +22655,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="348" spans="1:23" ht="72" customHeight="1">
+    <row r="348" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="6">
         <v>336</v>
       </c>
@@ -22687,7 +22696,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="349" spans="1:23" ht="72" customHeight="1">
+    <row r="349" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="6">
         <v>337</v>
       </c>
@@ -22728,7 +22737,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="350" spans="1:23" ht="72" customHeight="1">
+    <row r="350" spans="1:23" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="6">
         <v>338</v>
       </c>
@@ -22769,7 +22778,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="351" spans="1:23" ht="15.75">
+    <row r="351" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A351" s="29"/>
       <c r="B351" s="29"/>
       <c r="C351" s="29"/>
@@ -22797,7 +22806,7 @@
       </c>
       <c r="W351" s="29"/>
     </row>
-    <row r="352" spans="1:23" ht="15.75">
+    <row r="352" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A352" s="4"/>
       <c r="B352" s="4"/>
       <c r="C352" s="4"/>
@@ -22822,7 +22831,7 @@
       <c r="V352" s="4"/>
       <c r="W352" s="4"/>
     </row>
-    <row r="353" spans="1:23" ht="15.75">
+    <row r="353" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A353" s="4"/>
       <c r="B353" s="4"/>
       <c r="C353" s="4"/>
@@ -22847,7 +22856,7 @@
       <c r="V353" s="4"/>
       <c r="W353" s="4"/>
     </row>
-    <row r="354" spans="1:23" ht="15.75">
+    <row r="354" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A354" s="4"/>
       <c r="B354" s="4"/>
       <c r="C354" s="4"/>
@@ -22872,7 +22881,7 @@
       <c r="V354" s="4"/>
       <c r="W354" s="4"/>
     </row>
-    <row r="355" spans="1:23" ht="15.75">
+    <row r="355" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A355" s="4"/>
       <c r="B355" s="4"/>
       <c r="C355" s="4"/>
@@ -22897,7 +22906,7 @@
       <c r="V355" s="4"/>
       <c r="W355" s="4"/>
     </row>
-    <row r="356" spans="1:23" ht="15.75">
+    <row r="356" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A356" s="4"/>
       <c r="B356" s="4"/>
       <c r="C356" s="4"/>

</xml_diff>

<commit_message>
update: format excel dataset
</commit_message>
<xml_diff>
--- a/(UPDATE 2) DATA TUMBUHAN TERBARU.xlsx
+++ b/(UPDATE 2) DATA TUMBUHAN TERBARU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dev\laragon\www\botanica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9536290-B4A1-48F5-B4AE-A485401862A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6BF966-BD25-4BF1-B757-8D2D40A31239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ADBDB189-F3D4-457D-8897-29178EA9F1B5}"/>
+    <workbookView xWindow="0" yWindow="-105" windowWidth="29040" windowHeight="15705" xr2:uid="{ADBDB189-F3D4-457D-8897-29178EA9F1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Tumbuhan" sheetId="1" r:id="rId1"/>
@@ -5193,7 +5193,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5227,6 +5227,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5286,7 +5292,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5409,6 +5415,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5417,6 +5426,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA9D08E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5727,8 +5741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BE4F62-6877-4DC0-ABE6-E26131F42661}">
   <dimension ref="A1:X356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5787,7 +5801,7 @@
       <c r="M1" s="12" t="s">
         <v>1678</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="42" t="s">
         <v>1679</v>
       </c>
       <c r="O1" s="12" t="s">

</xml_diff>